<commit_message>
Status updated for 31st march 2020
Learning Git Commands
</commit_message>
<xml_diff>
--- a/Daily Status update Report 2803 (1) (1).xlsx
+++ b/Daily Status update Report 2803 (1) (1).xlsx
@@ -701,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3593,7 +3593,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3815,10 +3815,10 @@
         <v>15</v>
       </c>
       <c r="E13" s="18">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="F13" s="19">
-        <v>0.70833333333333337</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>89</v>

</xml_diff>